<commit_message>
rebuild file, modify cluster name and component name: outcomes/Bureaucratic Efficiency
</commit_message>
<xml_diff>
--- a/DII 4.0 Evolution Rebuild 240604.xlsx
+++ b/DII 4.0 Evolution Rebuild 240604.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xniu02\Desktop\DII 4.0 Index Construction 240319\DII 4.0 Index Construction 240610 - all updates - git - full\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4832F7-0C7D-4837-B3CE-A0C3C913CDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECD7D2F-DBBB-40B2-BB35-B7B02F3659D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="-15345" windowWidth="27795" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4365" yWindow="-15360" windowWidth="23595" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IndicatorInfo" sheetId="1" r:id="rId1"/>
@@ -1001,9 +1001,6 @@
     <t>crime</t>
   </si>
   <si>
-    <t>Bureaucracy</t>
-  </si>
-  <si>
     <t>Tax revenues as a share of GDP</t>
   </si>
   <si>
@@ -1412,9 +1409,6 @@
     <t>Value Capture</t>
   </si>
   <si>
-    <t>Output</t>
-  </si>
-  <si>
     <t>ict_serv_expo</t>
   </si>
   <si>
@@ -1617,6 +1611,12 @@
   </si>
   <si>
     <t>vc_ai_compute</t>
+  </si>
+  <si>
+    <t>Outcomes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bureaucratic Efficiency </t>
   </si>
 </sst>
 </file>
@@ -1961,8 +1961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="75" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3448,7 +3448,7 @@
     </row>
     <row r="28" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>93</v>
@@ -3463,7 +3463,7 @@
         <v>2023</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>91</v>
@@ -3650,7 +3650,7 @@
     </row>
     <row r="32" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>93</v>
@@ -3665,7 +3665,7 @@
         <v>2023</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>91</v>
@@ -3752,7 +3752,7 @@
     </row>
     <row r="34" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>93</v>
@@ -3767,7 +3767,7 @@
         <v>2023</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>91</v>
@@ -8124,10 +8124,10 @@
     </row>
     <row r="115" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>305</v>
+        <v>510</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>288</v>
@@ -8139,10 +8139,10 @@
         <v>2022</v>
       </c>
       <c r="F115" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="G115" s="4" t="s">
         <v>307</v>
-      </c>
-      <c r="G115" s="4" t="s">
-        <v>308</v>
       </c>
       <c r="H115" s="4"/>
       <c r="I115" s="4">
@@ -8172,10 +8172,10 @@
     </row>
     <row r="116" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>305</v>
+        <v>510</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>288</v>
@@ -8187,7 +8187,7 @@
         <v>2020</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G116" s="4" t="s">
         <v>291</v>
@@ -8230,10 +8230,10 @@
     </row>
     <row r="117" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>305</v>
+        <v>510</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>288</v>
@@ -8245,7 +8245,7 @@
         <v>2023</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G117" s="4" t="s">
         <v>91</v>
@@ -8280,13 +8280,13 @@
     </row>
     <row r="118" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B118" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="C118" s="4" t="s">
         <v>314</v>
-      </c>
-      <c r="C118" s="4" t="s">
-        <v>315</v>
       </c>
       <c r="D118" s="4" t="s">
         <v>289</v>
@@ -8295,7 +8295,7 @@
         <v>2022</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G118" s="4" t="s">
         <v>75</v>
@@ -8334,13 +8334,13 @@
     </row>
     <row r="119" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B119" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C119" s="4" t="s">
         <v>314</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>315</v>
       </c>
       <c r="D119" s="4" t="s">
         <v>289</v>
@@ -8349,7 +8349,7 @@
         <v>2019</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G119" s="4" t="s">
         <v>98</v>
@@ -8388,13 +8388,13 @@
     </row>
     <row r="120" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B120" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="B120" s="4" t="s">
-        <v>320</v>
-      </c>
       <c r="C120" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D120" s="4" t="s">
         <v>289</v>
@@ -8403,10 +8403,10 @@
         <v>2021</v>
       </c>
       <c r="F120" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="G120" s="4" t="s">
         <v>321</v>
-      </c>
-      <c r="G120" s="4" t="s">
-        <v>322</v>
       </c>
       <c r="H120" s="4" t="s">
         <v>23</v>
@@ -8446,13 +8446,13 @@
     </row>
     <row r="121" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D121" s="4" t="s">
         <v>289</v>
@@ -8461,7 +8461,7 @@
         <v>2022</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G121" s="4" t="s">
         <v>58</v>
@@ -8500,13 +8500,13 @@
     </row>
     <row r="122" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D122" s="4" t="s">
         <v>289</v>
@@ -8515,7 +8515,7 @@
         <v>2022</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G122" s="4" t="s">
         <v>58</v>
@@ -8554,13 +8554,13 @@
     </row>
     <row r="123" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D123" s="4" t="s">
         <v>289</v>
@@ -8569,7 +8569,7 @@
         <v>2022</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G123" s="4" t="s">
         <v>58</v>
@@ -8608,13 +8608,13 @@
     </row>
     <row r="124" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D124" s="4" t="s">
         <v>289</v>
@@ -8623,7 +8623,7 @@
         <v>2022</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G124" s="4" t="s">
         <v>58</v>
@@ -8662,13 +8662,13 @@
     </row>
     <row r="125" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D125" s="4" t="s">
         <v>289</v>
@@ -8677,7 +8677,7 @@
         <v>2022</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G125" s="4" t="s">
         <v>58</v>
@@ -8716,13 +8716,13 @@
     </row>
     <row r="126" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B126" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="B126" s="4" t="s">
-        <v>334</v>
-      </c>
       <c r="C126" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D126" s="4" t="s">
         <v>289</v>
@@ -8731,7 +8731,7 @@
         <v>2019</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G126" s="4" t="s">
         <v>98</v>
@@ -8770,13 +8770,13 @@
     </row>
     <row r="127" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D127" s="4" t="s">
         <v>289</v>
@@ -8785,10 +8785,10 @@
         <v>2022</v>
       </c>
       <c r="F127" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="G127" s="4" t="s">
         <v>337</v>
-      </c>
-      <c r="G127" s="4" t="s">
-        <v>338</v>
       </c>
       <c r="H127" s="4"/>
       <c r="I127" s="4">
@@ -8820,13 +8820,13 @@
     </row>
     <row r="128" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D128" s="4" t="s">
         <v>289</v>
@@ -8835,7 +8835,7 @@
         <v>2020</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G128" s="4" t="s">
         <v>58</v>
@@ -8874,13 +8874,13 @@
     </row>
     <row r="129" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D129" s="4" t="s">
         <v>289</v>
@@ -8889,10 +8889,10 @@
         <v>2022</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G129" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H129" s="4"/>
       <c r="I129" s="4">
@@ -8922,13 +8922,13 @@
     </row>
     <row r="130" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B130" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="C130" s="4" t="s">
         <v>342</v>
-      </c>
-      <c r="C130" s="4" t="s">
-        <v>343</v>
       </c>
       <c r="D130" s="4" t="s">
         <v>289</v>
@@ -8937,10 +8937,10 @@
         <v>2022</v>
       </c>
       <c r="F130" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="G130" s="4" t="s">
         <v>344</v>
-      </c>
-      <c r="G130" s="4" t="s">
-        <v>345</v>
       </c>
       <c r="H130" s="4" t="s">
         <v>28</v>
@@ -8976,13 +8976,13 @@
     </row>
     <row r="131" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B131" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C131" s="4" t="s">
         <v>342</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>343</v>
       </c>
       <c r="D131" s="4" t="s">
         <v>289</v>
@@ -8991,10 +8991,10 @@
         <v>2022</v>
       </c>
       <c r="F131" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="G131" s="4" t="s">
         <v>347</v>
-      </c>
-      <c r="G131" s="4" t="s">
-        <v>348</v>
       </c>
       <c r="H131" s="4" t="s">
         <v>28</v>
@@ -9030,13 +9030,13 @@
     </row>
     <row r="132" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B132" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C132" s="4" t="s">
         <v>342</v>
-      </c>
-      <c r="C132" s="4" t="s">
-        <v>343</v>
       </c>
       <c r="D132" s="4" t="s">
         <v>289</v>
@@ -9045,7 +9045,7 @@
         <v>2021</v>
       </c>
       <c r="F132" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G132" s="4" t="s">
         <v>27</v>
@@ -9084,13 +9084,13 @@
     </row>
     <row r="133" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B133" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C133" s="4" t="s">
         <v>342</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>343</v>
       </c>
       <c r="D133" s="4" t="s">
         <v>289</v>
@@ -9099,7 +9099,7 @@
         <v>2021</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G133" s="4" t="s">
         <v>27</v>
@@ -9138,13 +9138,13 @@
     </row>
     <row r="134" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B134" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C134" s="4" t="s">
         <v>342</v>
-      </c>
-      <c r="C134" s="4" t="s">
-        <v>343</v>
       </c>
       <c r="D134" s="4" t="s">
         <v>289</v>
@@ -9153,7 +9153,7 @@
         <v>2021</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G134" s="4" t="s">
         <v>27</v>
@@ -9192,13 +9192,13 @@
     </row>
     <row r="135" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B135" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C135" s="4" t="s">
         <v>342</v>
-      </c>
-      <c r="C135" s="4" t="s">
-        <v>343</v>
       </c>
       <c r="D135" s="4" t="s">
         <v>289</v>
@@ -9207,10 +9207,10 @@
         <v>2023</v>
       </c>
       <c r="F135" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="G135" s="4" t="s">
         <v>356</v>
-      </c>
-      <c r="G135" s="4" t="s">
-        <v>357</v>
       </c>
       <c r="H135" s="4" t="s">
         <v>23</v>
@@ -9244,13 +9244,13 @@
     </row>
     <row r="136" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B136" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="B136" s="4" t="s">
-        <v>359</v>
-      </c>
       <c r="C136" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D136" s="4" t="s">
         <v>289</v>
@@ -9259,10 +9259,10 @@
         <v>2020</v>
       </c>
       <c r="F136" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="G136" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="G136" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="H136" s="4" t="s">
         <v>23</v>
@@ -9294,13 +9294,13 @@
     </row>
     <row r="137" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D137" s="4" t="s">
         <v>289</v>
@@ -9309,10 +9309,10 @@
         <v>2022</v>
       </c>
       <c r="F137" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="G137" s="4" t="s">
         <v>363</v>
-      </c>
-      <c r="G137" s="4" t="s">
-        <v>364</v>
       </c>
       <c r="H137" s="4" t="s">
         <v>28</v>
@@ -9350,13 +9350,13 @@
     </row>
     <row r="138" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D138" s="4" t="s">
         <v>289</v>
@@ -9365,7 +9365,7 @@
         <v>2021</v>
       </c>
       <c r="F138" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G138" s="4" t="s">
         <v>27</v>
@@ -9404,13 +9404,13 @@
     </row>
     <row r="139" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D139" s="4" t="s">
         <v>289</v>
@@ -9419,7 +9419,7 @@
         <v>2021</v>
       </c>
       <c r="F139" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G139" s="4" t="s">
         <v>27</v>
@@ -9458,22 +9458,22 @@
     </row>
     <row r="140" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="B140" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="C140" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="C140" s="4" t="s">
+      <c r="D140" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D140" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E140" s="4">
         <v>2019</v>
       </c>
       <c r="F140" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G140" s="4" t="s">
         <v>98</v>
@@ -9512,22 +9512,22 @@
     </row>
     <row r="141" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B141" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C141" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="C141" s="4" t="s">
+      <c r="D141" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D141" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E141" s="4">
         <v>2019</v>
       </c>
       <c r="F141" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G141" s="4" t="s">
         <v>98</v>
@@ -9566,22 +9566,22 @@
     </row>
     <row r="142" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B142" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C142" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="C142" s="4" t="s">
+      <c r="D142" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D142" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E142" s="4">
         <v>2022</v>
       </c>
       <c r="F142" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G142" s="4" t="s">
         <v>80</v>
@@ -9605,10 +9605,10 @@
         <v>29</v>
       </c>
       <c r="N142" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="O142" s="4" t="s">
         <v>378</v>
-      </c>
-      <c r="O142" s="4" t="s">
-        <v>379</v>
       </c>
       <c r="P142" s="4"/>
       <c r="Q142" s="4"/>
@@ -9624,25 +9624,25 @@
     </row>
     <row r="143" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B143" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C143" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="C143" s="4" t="s">
+      <c r="D143" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D143" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E143" s="4">
         <v>2022</v>
       </c>
       <c r="F143" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="G143" s="4" t="s">
         <v>381</v>
-      </c>
-      <c r="G143" s="4" t="s">
-        <v>382</v>
       </c>
       <c r="H143" s="4" t="s">
         <v>28</v>
@@ -9663,10 +9663,10 @@
         <v>29</v>
       </c>
       <c r="N143" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="O143" s="4" t="s">
         <v>378</v>
-      </c>
-      <c r="O143" s="4" t="s">
-        <v>379</v>
       </c>
       <c r="P143" s="4"/>
       <c r="Q143" s="4"/>
@@ -9682,22 +9682,22 @@
     </row>
     <row r="144" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B144" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C144" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="C144" s="4" t="s">
+      <c r="D144" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D144" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E144" s="4">
         <v>2022</v>
       </c>
       <c r="F144" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G144" s="4" t="s">
         <v>27</v>
@@ -9736,25 +9736,25 @@
     </row>
     <row r="145" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B145" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C145" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="C145" s="4" t="s">
+      <c r="D145" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D145" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E145" s="4">
         <v>2023</v>
       </c>
       <c r="F145" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="G145" s="4" t="s">
         <v>386</v>
-      </c>
-      <c r="G145" s="4" t="s">
-        <v>387</v>
       </c>
       <c r="H145" s="4" t="s">
         <v>23</v>
@@ -9771,7 +9771,7 @@
         <v>155</v>
       </c>
       <c r="N145" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="O145" s="4"/>
       <c r="P145" s="4"/>
@@ -9788,25 +9788,25 @@
     </row>
     <row r="146" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" s="4" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B146" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C146" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="C146" s="4" t="s">
+      <c r="D146" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D146" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E146" s="4">
         <v>2023</v>
       </c>
       <c r="F146" s="4" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="G146" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H146" s="4"/>
       <c r="I146" s="4">
@@ -9836,22 +9836,22 @@
     </row>
     <row r="147" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B147" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="B147" s="4" t="s">
-        <v>389</v>
-      </c>
       <c r="C147" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D147" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D147" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E147" s="4">
         <v>2020</v>
       </c>
       <c r="F147" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G147" s="4" t="s">
         <v>27</v>
@@ -9888,22 +9888,22 @@
     </row>
     <row r="148" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C148" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D148" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D148" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E148" s="4">
         <v>2020</v>
       </c>
       <c r="F148" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G148" s="4" t="s">
         <v>27</v>
@@ -9940,23 +9940,23 @@
     </row>
     <row r="149" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C149" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D149" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D149" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E149" s="4"/>
       <c r="F149" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="G149" s="4" t="s">
         <v>394</v>
-      </c>
-      <c r="G149" s="4" t="s">
-        <v>395</v>
       </c>
       <c r="H149" s="4" t="s">
         <v>28</v>
@@ -9992,22 +9992,22 @@
     </row>
     <row r="150" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="B150" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="B150" s="4" t="s">
-        <v>397</v>
-      </c>
       <c r="C150" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D150" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D150" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E150" s="4">
         <v>2019</v>
       </c>
       <c r="F150" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G150" s="4" t="s">
         <v>98</v>
@@ -10046,22 +10046,22 @@
     </row>
     <row r="151" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C151" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D151" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D151" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E151" s="4">
         <v>2019</v>
       </c>
       <c r="F151" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G151" s="4" t="s">
         <v>98</v>
@@ -10100,22 +10100,22 @@
     </row>
     <row r="152" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C152" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D152" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D152" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E152" s="4">
         <v>2022</v>
       </c>
       <c r="F152" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G152" s="4" t="s">
         <v>91</v>
@@ -10132,7 +10132,7 @@
       <c r="K152" s="4"/>
       <c r="L152" s="4"/>
       <c r="M152" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="N152" s="4"/>
       <c r="O152" s="4"/>
@@ -10150,22 +10150,22 @@
     </row>
     <row r="153" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C153" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D153" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D153" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E153" s="4">
         <v>2019</v>
       </c>
       <c r="F153" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G153" s="4" t="s">
         <v>98</v>
@@ -10204,25 +10204,25 @@
     </row>
     <row r="154" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C154" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D154" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D154" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E154" s="4">
         <v>2022</v>
       </c>
       <c r="F154" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G154" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H154" s="4" t="s">
         <v>23</v>
@@ -10254,25 +10254,25 @@
     </row>
     <row r="155" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C155" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D155" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="D155" s="4" t="s">
-        <v>372</v>
       </c>
       <c r="E155" s="4">
         <v>2022</v>
       </c>
       <c r="F155" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G155" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H155" s="4" t="s">
         <v>23</v>
@@ -10304,22 +10304,22 @@
     </row>
     <row r="156" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="B156" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="C156" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="C156" s="4" t="s">
-        <v>412</v>
-      </c>
       <c r="D156" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E156" s="4">
         <v>2019</v>
       </c>
       <c r="F156" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G156" s="4" t="s">
         <v>98</v>
@@ -10358,22 +10358,22 @@
     </row>
     <row r="157" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B157" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="C157" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="C157" s="4" t="s">
-        <v>412</v>
-      </c>
       <c r="D157" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E157" s="4">
         <v>2019</v>
       </c>
       <c r="F157" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G157" s="4" t="s">
         <v>98</v>
@@ -10412,22 +10412,22 @@
     </row>
     <row r="158" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B158" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="C158" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="C158" s="4" t="s">
-        <v>412</v>
-      </c>
       <c r="D158" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E158" s="4">
         <v>2022</v>
       </c>
       <c r="F158" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G158" s="4" t="s">
         <v>80</v>
@@ -10466,22 +10466,22 @@
     </row>
     <row r="159" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="B159" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="B159" s="4" t="s">
-        <v>419</v>
-      </c>
       <c r="C159" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E159" s="4">
         <v>2019</v>
       </c>
       <c r="F159" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G159" s="4" t="s">
         <v>98</v>
@@ -10520,22 +10520,22 @@
     </row>
     <row r="160" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E160" s="4">
         <v>2019</v>
       </c>
       <c r="F160" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G160" s="4" t="s">
         <v>98</v>
@@ -10574,22 +10574,22 @@
     </row>
     <row r="161" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E161" s="4">
         <v>2021</v>
       </c>
       <c r="F161" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G161" s="4" t="s">
         <v>27</v>
@@ -10606,7 +10606,7 @@
       <c r="K161" s="4"/>
       <c r="L161" s="4"/>
       <c r="M161" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="N161" s="4"/>
       <c r="O161" s="4"/>
@@ -10624,25 +10624,25 @@
     </row>
     <row r="162" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E162" s="4">
         <v>2021</v>
       </c>
       <c r="F162" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="G162" s="4" t="s">
         <v>426</v>
-      </c>
-      <c r="G162" s="4" t="s">
-        <v>427</v>
       </c>
       <c r="H162" s="4" t="s">
         <v>23</v>
@@ -10656,10 +10656,10 @@
       <c r="K162" s="4"/>
       <c r="L162" s="4"/>
       <c r="M162" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="N162" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="O162" s="4"/>
       <c r="P162" s="4"/>
@@ -10676,22 +10676,22 @@
     </row>
     <row r="163" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E163" s="4">
         <v>2019</v>
       </c>
       <c r="F163" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G163" s="4" t="s">
         <v>98</v>
@@ -10730,25 +10730,25 @@
     </row>
     <row r="164" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E164" s="4">
         <v>2021</v>
       </c>
       <c r="F164" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G164" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H164" s="4" t="s">
         <v>28</v>
@@ -10784,25 +10784,25 @@
     </row>
     <row r="165" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E165" s="4">
         <v>2021</v>
       </c>
       <c r="F165" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G165" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H165" s="4" t="s">
         <v>28</v>
@@ -10838,25 +10838,25 @@
     </row>
     <row r="166" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E166" s="4">
         <v>2023</v>
       </c>
       <c r="F166" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="G166" s="4" t="s">
         <v>435</v>
-      </c>
-      <c r="G166" s="4" t="s">
-        <v>436</v>
       </c>
       <c r="H166" s="4" t="s">
         <v>23</v>
@@ -10888,25 +10888,25 @@
     </row>
     <row r="167" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E167" s="4">
         <v>2022</v>
       </c>
       <c r="F167" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="G167" s="4" t="s">
         <v>438</v>
-      </c>
-      <c r="G167" s="4" t="s">
-        <v>439</v>
       </c>
       <c r="H167" s="4" t="s">
         <v>23</v>
@@ -10938,22 +10938,22 @@
     </row>
     <row r="168" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="B168" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="B168" s="4" t="s">
-        <v>441</v>
-      </c>
       <c r="C168" s="4" t="s">
-        <v>442</v>
+        <v>509</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E168" s="4">
         <v>2022</v>
       </c>
       <c r="F168" s="4" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="G168" s="4" t="s">
         <v>27</v>
@@ -10970,7 +10970,7 @@
       <c r="K168" s="4"/>
       <c r="L168" s="4"/>
       <c r="M168" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="N168" s="4"/>
       <c r="O168" s="4"/>
@@ -10988,22 +10988,22 @@
     </row>
     <row r="169" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" s="4" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>442</v>
+        <v>509</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E169" s="4">
         <v>2022</v>
       </c>
       <c r="F169" s="4" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="G169" s="4" t="s">
         <v>27</v>
@@ -11027,10 +11027,10 @@
         <v>29</v>
       </c>
       <c r="N169" s="9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="O169" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="P169" s="4"/>
       <c r="Q169" s="4"/>
@@ -11046,22 +11046,22 @@
     </row>
     <row r="170" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="4" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>442</v>
+        <v>509</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E170" s="4">
         <v>2021</v>
       </c>
       <c r="F170" s="4" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G170" s="4" t="s">
         <v>27</v>
@@ -11100,22 +11100,22 @@
     </row>
     <row r="171" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" s="4" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>442</v>
+        <v>509</v>
       </c>
       <c r="D171" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E171" s="4">
         <v>2021</v>
       </c>
       <c r="F171" s="4" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G171" s="4" t="s">
         <v>27</v>
@@ -11154,22 +11154,22 @@
     </row>
     <row r="172" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" s="4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>442</v>
+        <v>509</v>
       </c>
       <c r="D172" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E172" s="4">
         <v>2021</v>
       </c>
       <c r="F172" s="4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G172" s="4" t="s">
         <v>27</v>
@@ -11193,10 +11193,10 @@
         <v>29</v>
       </c>
       <c r="N172" s="9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="O172" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="P172" s="4"/>
       <c r="Q172" s="4"/>
@@ -11212,19 +11212,19 @@
     </row>
     <row r="173" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" s="4" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>442</v>
+        <v>509</v>
       </c>
       <c r="D173" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F173" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="G173" s="4" t="s">
         <v>27</v>
@@ -11252,22 +11252,22 @@
     </row>
     <row r="174" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" s="4" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>442</v>
+        <v>509</v>
       </c>
       <c r="D174" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E174" s="4">
         <v>2022</v>
       </c>
       <c r="F174" s="4" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="G174" s="4" t="s">
         <v>41</v>
@@ -11306,25 +11306,25 @@
     </row>
     <row r="175" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" s="4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>442</v>
+        <v>509</v>
       </c>
       <c r="D175" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E175" s="4">
         <v>2021</v>
       </c>
       <c r="F175" s="4" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="G175" s="4" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H175" s="4" t="s">
         <v>28</v>
@@ -11362,22 +11362,22 @@
     </row>
     <row r="176" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" s="4" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>442</v>
+        <v>509</v>
       </c>
       <c r="D176" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E176" s="4">
         <v>2020</v>
       </c>
       <c r="F176" s="4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="G176" s="4" t="s">
         <v>27</v>
@@ -11420,22 +11420,22 @@
     </row>
     <row r="177" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="4" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D177" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E177" s="4">
         <v>2023</v>
       </c>
       <c r="F177" s="4" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="G177" s="4" t="s">
         <v>80</v>
@@ -11448,7 +11448,7 @@
       <c r="K177" s="4"/>
       <c r="L177" s="4"/>
       <c r="M177" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="N177" s="4"/>
       <c r="O177" s="4"/>
@@ -11466,22 +11466,22 @@
     </row>
     <row r="178" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" s="4" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D178" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E178" s="4">
         <v>2023</v>
       </c>
       <c r="F178" s="4" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="G178" s="4" t="s">
         <v>80</v>
@@ -11494,7 +11494,7 @@
       <c r="K178" s="4"/>
       <c r="L178" s="4"/>
       <c r="M178" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="N178" s="4"/>
       <c r="O178" s="4"/>
@@ -11512,22 +11512,22 @@
     </row>
     <row r="179" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D179" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E179" s="4">
         <v>2023</v>
       </c>
       <c r="F179" s="4" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G179" s="4" t="s">
         <v>80</v>
@@ -11540,7 +11540,7 @@
       <c r="K179" s="4"/>
       <c r="L179" s="4"/>
       <c r="M179" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="N179" s="4"/>
       <c r="O179" s="4"/>
@@ -11558,22 +11558,22 @@
     </row>
     <row r="180" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="4" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D180" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E180" s="4">
         <v>2022</v>
       </c>
       <c r="F180" s="4" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="G180" s="4" t="s">
         <v>80</v>
@@ -11586,7 +11586,7 @@
       <c r="K180" s="4"/>
       <c r="L180" s="4"/>
       <c r="M180" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="N180" s="4"/>
       <c r="O180" s="4"/>
@@ -11604,22 +11604,22 @@
     </row>
     <row r="181" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="4" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D181" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E181" s="4">
         <v>2022</v>
       </c>
       <c r="F181" s="4" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="G181" s="4" t="s">
         <v>80</v>
@@ -11632,7 +11632,7 @@
       <c r="K181" s="4"/>
       <c r="L181" s="4"/>
       <c r="M181" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="N181" s="4"/>
       <c r="O181" s="4"/>
@@ -11650,22 +11650,22 @@
     </row>
     <row r="182" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="4" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E182" s="4">
         <v>2022</v>
       </c>
       <c r="F182" s="4" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="G182" s="4" t="s">
         <v>80</v>
@@ -11678,7 +11678,7 @@
       <c r="K182" s="4"/>
       <c r="L182" s="4"/>
       <c r="M182" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="N182" s="4"/>
       <c r="O182" s="4"/>
@@ -11696,25 +11696,25 @@
     </row>
     <row r="183" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="4" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D183" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E183" s="4">
         <v>2022</v>
       </c>
       <c r="F183" s="4" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G183" s="4" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H183" s="4" t="s">
         <v>23</v>
@@ -11724,7 +11724,7 @@
       <c r="K183" s="4"/>
       <c r="L183" s="4"/>
       <c r="M183" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="N183" s="4"/>
       <c r="O183" s="4"/>
@@ -11742,16 +11742,16 @@
     </row>
     <row r="184" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" s="4" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D184" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E184" s="4">
         <v>2022</v>
@@ -11770,7 +11770,7 @@
       <c r="K184" s="4"/>
       <c r="L184" s="4"/>
       <c r="M184" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="N184" s="4"/>
       <c r="O184" s="4"/>
@@ -11788,22 +11788,22 @@
     </row>
     <row r="185" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="4" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D185" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E185" s="4">
         <v>2023</v>
       </c>
       <c r="F185" s="4" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G185" s="4" t="s">
         <v>80</v>
@@ -11816,7 +11816,7 @@
       <c r="K185" s="4"/>
       <c r="L185" s="4"/>
       <c r="M185" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="N185" s="4"/>
       <c r="O185" s="4"/>
@@ -34692,7 +34692,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -34713,10 +34715,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -34724,7 +34726,7 @@
         <v>121</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>191</v>
@@ -34741,7 +34743,7 @@
         <v>121</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>205</v>
@@ -34758,7 +34760,7 @@
         <v>121</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>214</v>
@@ -34846,7 +34848,7 @@
         <v>143</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
@@ -34863,7 +34865,7 @@
         <v>143</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
@@ -34877,7 +34879,7 @@
         <v>121</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>136</v>
@@ -34894,10 +34896,10 @@
         <v>121</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D12" s="6">
         <v>1</v>
@@ -34911,7 +34913,7 @@
         <v>121</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>131</v>
@@ -34925,13 +34927,13 @@
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D14" s="6">
         <v>1</v>
@@ -34942,13 +34944,13 @@
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D15" s="6">
         <v>1</v>
@@ -34959,13 +34961,13 @@
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D16" s="6">
         <v>1</v>
@@ -34976,13 +34978,13 @@
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>442</v>
+        <v>371</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>509</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D17" s="6">
         <v>1</v>
@@ -34993,13 +34995,13 @@
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>442</v>
+        <v>371</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>509</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D18" s="6">
         <v>1</v>
@@ -35010,13 +35012,13 @@
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
@@ -35027,13 +35029,13 @@
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D20" s="6">
         <v>1</v>
@@ -35047,10 +35049,10 @@
         <v>289</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
@@ -35064,10 +35066,10 @@
         <v>289</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D22" s="6">
         <v>1</v>
@@ -35081,10 +35083,10 @@
         <v>289</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>491</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>305</v>
+        <v>489</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>510</v>
       </c>
       <c r="D23" s="6">
         <v>1</v>
@@ -35098,10 +35100,10 @@
         <v>289</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D24" s="6">
         <v>0.75</v>
@@ -35115,10 +35117,10 @@
         <v>289</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D25" s="6">
         <v>1</v>
@@ -35132,10 +35134,10 @@
         <v>289</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>493</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>495</v>
       </c>
       <c r="D26" s="6">
         <v>1</v>
@@ -35149,10 +35151,10 @@
         <v>289</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D27" s="6">
         <v>1.25</v>
@@ -35288,7 +35290,7 @@
         <v>78</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D35" s="6">
         <v>1</v>
@@ -36288,11 +36290,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="26" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" customWidth="1"/>
+    <col min="2" max="2" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="26" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -36303,10 +36309,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -36314,7 +36320,7 @@
         <v>121</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C2" s="6">
         <v>0.5</v>
@@ -36356,7 +36362,7 @@
         <v>121</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C5" s="6">
         <v>1.25</v>
@@ -36367,10 +36373,10 @@
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C6" s="6">
         <v>1</v>
@@ -36381,10 +36387,10 @@
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>442</v>
+        <v>371</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>509</v>
       </c>
       <c r="C7" s="6">
         <v>1</v>
@@ -36395,10 +36401,10 @@
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C8" s="6">
         <v>0.75</v>
@@ -36412,7 +36418,7 @@
         <v>289</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
@@ -36426,7 +36432,7 @@
         <v>289</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C10" s="6">
         <v>0.5</v>
@@ -36440,7 +36446,7 @@
         <v>289</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C11" s="6">
         <v>1</v>
@@ -37500,7 +37506,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -37513,7 +37519,7 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B3" s="6">
         <v>1</v>

</xml_diff>